<commit_message>
Fixed a bug where there would be an extra sheet when creating a new workbook. Updated the readme.
</commit_message>
<xml_diff>
--- a/carEvalsAutomated.xlsx
+++ b/carEvalsAutomated.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Car Evaluations" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -346,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,7 +508,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2019-12-29 19:21:52.275477</t>
+          <t>2019-12-29 19:32:08.884654</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -521,52 +520,52 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2017 Ford Mustang GT</t>
+          <t>2017 Honda Accord LX</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$25,260</t>
+          <t>$15,995</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">16,392 miles </t>
+          <t xml:space="preserve">26,832 miles </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vienna, VA </t>
+          <t xml:space="preserve">Falls Church, VA </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Blue</t>
+          <t>Unspecified</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Black</t>
+          <t>Unspecified</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>RWD</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Automatic</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Coupe</t>
+          <t>Sedan</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>8 Cyl 5.0 L</t>
+          <t>4 Cyl 2.4 L</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -576,54 +575,54 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>15/25</t>
+          <t>26/34</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>1FA6P8CFXH5249463</t>
+          <t>1HGCR2F35HA094805</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>IP2997A</t>
+          <t>HP4847</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2019-12-29 19:21:53.063157</t>
+          <t>2019-12-29 19:33:12.889521</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>https://www.carfax.com/vehicle/1FA6P8CFXH5249463</t>
+          <t>https://www.carfax.com/vehicle/1HGCR2F35HA094805</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2014 Ford Mustang</t>
+          <t>2016 Honda Accord Sport</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$15,000</t>
+          <t>$16,277</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">22,671 miles </t>
+          <t xml:space="preserve">28,474 miles </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Westminster, MD </t>
+          <t xml:space="preserve">Stafford, VA </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Gray</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -633,7 +632,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>RWD</t>
+          <t>FWD</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -643,12 +642,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Coupe</t>
+          <t>Sedan</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>6 Cyl 3.7 L</t>
+          <t>4 Cyl 2.4 L</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -658,49 +657,113 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>19/30</t>
+          <t>26/34</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>1ZVBP8AM1E5209582</t>
+          <t>1HGCR2F52GA125671</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>MU209582</t>
+          <t>125671</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2019-12-29 19:22:32.697683</t>
+          <t>2019-12-29 19:33:14.067253</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>https://www.carfax.com/vehicle/1ZVBP8AM1E5209582</t>
+          <t>https://www.carfax.com/vehicle/1HGCR2F52GA125671</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2015 Honda Accord EXL</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>$15,371</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">68,777 miles </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Germantown, MD </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>FWD</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Automatic</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Sedan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>6 Cyl 3.5 L</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Gasoline</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>21/31</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>1HGCR3F85FA011615</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>H191579B</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2019-12-29 19:34:34.986326</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>https://www.carfax.com/vehicle/1HGCR3F85FA011615</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
 </file>
</xml_diff>